<commit_message>
version 2 - all working
</commit_message>
<xml_diff>
--- a/DS_Game_Cards_Image_Record.xlsx
+++ b/DS_Game_Cards_Image_Record.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26914"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amzsu\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1166" documentId="8_{7FF596D7-E8B1-439C-B940-F71B3752A70E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58B6CECC-6283-4E4D-8F60-959B57734424}"/>
+  <xr:revisionPtr revIDLastSave="1192" documentId="8_{7FF596D7-E8B1-439C-B940-F71B3752A70E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8D1E522-7344-41C7-8570-9721769E3D9A}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{86E0261B-6764-4F8F-8021-EFB3FC3E72C8}"/>
   </bookViews>
@@ -252,7 +252,7 @@
     <t>Replay</t>
   </si>
   <si>
-    <t>Can the score be peformed without you there</t>
+    <t>Can the score be peformed without you there?</t>
   </si>
   <si>
     <t>https://live.staticflickr.com/4433/36912849980_08290105a6_k_d.jpg</t>
@@ -264,7 +264,7 @@
     <t>Wrong Language</t>
   </si>
   <si>
-    <t>The notation does not suit the aesthetic purpose of the music</t>
+    <t>The notation does not suit the aesthetic purpose of the music.</t>
   </si>
   <si>
     <t>https://live.staticflickr.com/4320/36139409192_6692562d45_k_d.jpg</t>
@@ -276,7 +276,7 @@
     <t>Rehearsal Marks</t>
   </si>
   <si>
-    <t>Important sections of the score are directly accessible for rehearsal &amp; repeating</t>
+    <t>Important sections of the score are directly accessible for rehearsal &amp; repeating.</t>
   </si>
   <si>
     <t>https://live.staticflickr.com/3053/3025559027_a23cea0973_k_d.jpg</t>
@@ -312,7 +312,7 @@
     <t>Timed Events</t>
   </si>
   <si>
-    <t>players have to be at the right place at the right time.</t>
+    <t>Players have to be at the right place at the right time.</t>
   </si>
   <si>
     <t>https://live.staticflickr.com/8334/8086529320_e220232e4d_k_d.jpg</t>
@@ -408,7 +408,7 @@
     <t>Getting Lost</t>
   </si>
   <si>
-    <t>How likely is it that players will wander in the wrong direction.</t>
+    <t>How likely is it that players will wander in the wrong direction?</t>
   </si>
   <si>
     <t>https://live.staticflickr.com/1516/26628931562_2bcdb0f71e_k_d.jpg</t>
@@ -444,7 +444,7 @@
     <t>Stimulus</t>
   </si>
   <si>
-    <t>How does your score offer differnt possibities and journeys?</t>
+    <t>How does your score offer different possibities and journeys?</t>
   </si>
   <si>
     <t>https://live.staticflickr.com/5069/5583561290_d2dbf1e346_k_d.jpg</t>
@@ -759,7 +759,7 @@
     <t>Noise</t>
   </si>
   <si>
-    <t>How does the performance environment impact the music.</t>
+    <t>How does the performance environment impact the music?</t>
   </si>
   <si>
     <t>https://live.staticflickr.com/1666/25398229984_e5274134ff_k_d.jpg</t>
@@ -1020,7 +1020,7 @@
     <t>Pleasure</t>
   </si>
   <si>
-    <t>Playful moods such as mischief, humour, wonder, thrill, reinforce the experience?</t>
+    <t>Playful moods such as mischief, humour, wonder, reinforce the experience?</t>
   </si>
   <si>
     <t>https://live.staticflickr.com/3057/3110322867_646ef605be_k_d.jpg</t>
@@ -1194,7 +1194,7 @@
     <t>Fuzzy Logic</t>
   </si>
   <si>
-    <t>How can AI or randomness enhance the score</t>
+    <t>How can AI or randomness enhance the score?</t>
   </si>
   <si>
     <t>Alternative Content</t>
@@ -1245,7 +1245,7 @@
     <t>Raul Pacheco-Vega</t>
   </si>
   <si>
-    <t>Lighting and Scenography</t>
+    <t>Lighting &amp; Scenography</t>
   </si>
   <si>
     <t>Can the score be enhanced with lighting and stage design?</t>
@@ -1272,7 +1272,7 @@
     <t>Dynamic Recordings</t>
   </si>
   <si>
-    <t>Can the recorded media be split into smallers chunks and randomised?</t>
+    <t>Can the recorded media be split into smaller chunks and randomised?</t>
   </si>
   <si>
     <t>https://live.staticflickr.com/3004/3058562807_e8a12f5b10_k_d.jpg</t>
@@ -1332,7 +1332,7 @@
     <t>Subjectivity</t>
   </si>
   <si>
-    <t>The purpose of the score is confused by the individual interpretation</t>
+    <t>The purpose of the score is confused by the individual interpretation.</t>
   </si>
   <si>
     <t>https://live.staticflickr.com/3507/3879128184_e96bc91d10_k_d.jpg</t>
@@ -1515,7 +1515,7 @@
     <t>Time And Form</t>
   </si>
   <si>
-    <t>Sections and paths through the score are indicated</t>
+    <t>Sections and paths through the score are indicated.</t>
   </si>
   <si>
     <t>Gimmicky Tech</t>
@@ -1608,7 +1608,7 @@
     <t>Tech Conductor</t>
   </si>
   <si>
-    <t>Software controls the sequencing og audio and/or visual material.</t>
+    <t>Software controls the sequencing of audio and/or visual material.</t>
   </si>
   <si>
     <t>Fitting Locations</t>
@@ -1693,7 +1693,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1725,7 +1725,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -1733,10 +1732,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1803,7 +1808,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -1817,6 +1822,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2163,8 +2169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0B9505E-DBBE-44C4-BC31-708A3D151DCD}">
   <dimension ref="A1:L154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="E113" sqref="E113"/>
+    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
+      <selection activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2448,7 +2454,7 @@
       <c r="B11">
         <v>2</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="12" t="s">
         <v>61</v>
       </c>
       <c r="D11" t="s">
@@ -2471,7 +2477,7 @@
       <c r="B12">
         <v>5</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="12" t="s">
         <v>65</v>
       </c>
       <c r="D12" t="s">
@@ -2586,7 +2592,7 @@
       <c r="B17">
         <v>1</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="11" t="s">
         <v>85</v>
       </c>
       <c r="D17" t="s">
@@ -2747,7 +2753,7 @@
       <c r="B24">
         <v>6</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="1" t="s">
         <v>113</v>
       </c>
       <c r="D24" t="s">
@@ -2816,7 +2822,7 @@
       <c r="B27">
         <v>2</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="12" t="s">
         <v>125</v>
       </c>
       <c r="D27" t="s">
@@ -3072,7 +3078,7 @@
       <c r="C38" t="s">
         <v>169</v>
       </c>
-      <c r="D38" s="12" t="s">
+      <c r="D38" s="11" t="s">
         <v>170</v>
       </c>
       <c r="E38" t="s">
@@ -3138,7 +3144,7 @@
       <c r="B41">
         <v>6</v>
       </c>
-      <c r="C41" s="12" t="s">
+      <c r="C41" s="11" t="s">
         <v>179</v>
       </c>
       <c r="D41" t="s">
@@ -3187,7 +3193,7 @@
       <c r="C43" t="s">
         <v>187</v>
       </c>
-      <c r="D43" s="12" t="s">
+      <c r="D43" s="11" t="s">
         <v>188</v>
       </c>
       <c r="E43" t="s">
@@ -3233,7 +3239,7 @@
       <c r="C45" t="s">
         <v>195</v>
       </c>
-      <c r="D45" s="11" t="s">
+      <c r="D45" s="13" t="s">
         <v>196</v>
       </c>
       <c r="E45" t="s">
@@ -3962,7 +3968,7 @@
       <c r="B78">
         <v>7</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C78" s="12" t="s">
         <v>317</v>
       </c>
       <c r="D78" t="s">
@@ -4307,7 +4313,7 @@
       <c r="B93">
         <v>4</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C93" s="1" t="s">
         <v>375</v>
       </c>
       <c r="D93" t="s">
@@ -4413,7 +4419,7 @@
       <c r="B98">
         <v>1</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C98" s="12" t="s">
         <v>393</v>
       </c>
       <c r="D98" t="s">
@@ -4459,7 +4465,7 @@
       <c r="B100">
         <v>4</v>
       </c>
-      <c r="C100" t="s">
+      <c r="C100" s="1" t="s">
         <v>401</v>
       </c>
       <c r="D100" t="s">
@@ -4588,7 +4594,7 @@
       <c r="B106">
         <v>4</v>
       </c>
-      <c r="C106" t="s">
+      <c r="C106" s="1" t="s">
         <v>421</v>
       </c>
       <c r="D106" t="s">
@@ -4977,7 +4983,7 @@
       <c r="B128">
         <v>6</v>
       </c>
-      <c r="C128" t="s">
+      <c r="C128" s="12" t="s">
         <v>482</v>
       </c>
       <c r="D128" t="s">
@@ -5196,7 +5202,7 @@
       <c r="B143">
         <v>2</v>
       </c>
-      <c r="C143" t="s">
+      <c r="C143" s="12" t="s">
         <v>513</v>
       </c>
       <c r="D143" t="s">
@@ -5512,12 +5518,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="cbbcf388-4be4-4cd6-9e4b-350ad5c5ef2f" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="63f57362-4c8e-4cde-8154-1d3ad19836ed">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5750,18 +5758,16 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="cbbcf388-4be4-4cd6-9e4b-350ad5c5ef2f" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="63f57362-4c8e-4cde-8154-1d3ad19836ed">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E50BC29-0B9C-4908-8DDB-4AD71D434C46}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{09FFAC7A-65E4-462C-8978-0935DD9F3D1C}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5769,5 +5775,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{09FFAC7A-65E4-462C-8978-0935DD9F3D1C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E50BC29-0B9C-4908-8DDB-4AD71D434C46}"/>
 </file>
</xml_diff>